<commit_message>
Updating as of class till 5th Sep
</commit_message>
<xml_diff>
--- a/DS_April_DEC/Data Science_Curriculum_Plan_DEC_APR.xlsx
+++ b/DS_April_DEC/Data Science_Curriculum_Plan_DEC_APR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training'\DS\EKeeda\DS_April_DEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training'\eKeeda\DS_April_DEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65886B1-DA31-4F1A-87DB-0A00FEEB9DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5876B-F60A-4ED8-B785-EE092796E0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="324">
   <si>
     <t>Modules</t>
   </si>
@@ -958,13 +958,61 @@
   </si>
   <si>
     <t>7:30-10:30</t>
+  </si>
+  <si>
+    <t>Thrusday</t>
+  </si>
+  <si>
+    <t>2 hrs 53 mins</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
+  </si>
+  <si>
+    <t>2 hrs 2 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 19 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 38 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 35 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 49 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 31 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 48 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 36 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 33 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 50 mins</t>
+  </si>
+  <si>
+    <t>2 hrs 55 mins</t>
+  </si>
+  <si>
+    <t>3 hrs 04 mins</t>
+  </si>
+  <si>
+    <t>8:00- 10:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1047,6 +1095,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1098,7 +1152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1264,11 +1318,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1360,16 +1474,59 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1389,54 +1546,33 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="19" fontId="13" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="13" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1660,7 +1796,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132:A133"/>
+      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1700,7 +1836,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
@@ -1709,37 +1845,37 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="35">
         <v>6</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="35" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="3">
         <v>1.2</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="3">
         <v>1.3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3">
@@ -1748,59 +1884,59 @@
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="35">
         <v>5</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="32" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="3">
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="3">
         <v>2.4</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="3">
         <v>2.5</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="32"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="3">
@@ -1809,68 +1945,68 @@
       <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="35">
         <v>6</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="3">
         <v>3.2</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="3">
         <v>3.3</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="3">
         <v>3.4</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="3">
         <v>3.5</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="3">
         <v>3.6</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="32"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="3">
@@ -1879,46 +2015,46 @@
       <c r="C17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="35">
         <v>4</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="3">
         <v>4.2</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="3">
         <v>4.3</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="35" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="3">
@@ -1927,70 +2063,70 @@
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="35">
         <v>6</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="35" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="3">
         <v>5.2</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="3">
         <v>5.3</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
     </row>
     <row r="24" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="3">
         <v>5.4</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="3">
         <v>5.5</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="3">
         <v>5.6</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="35" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3">
@@ -1999,37 +2135,37 @@
       <c r="C27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="31">
-        <v>3</v>
-      </c>
-      <c r="E27" s="34" t="s">
+      <c r="D27" s="35">
+        <v>3</v>
+      </c>
+      <c r="E27" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="3">
         <v>6.2</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="3">
         <v>6.3</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="32"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="3">
@@ -2041,10 +2177,10 @@
       <c r="D30" s="3">
         <v>3</v>
       </c>
-      <c r="E30" s="32"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="3">
         <v>7.2</v>
       </c>
@@ -2054,10 +2190,10 @@
       <c r="D31" s="3">
         <v>3</v>
       </c>
-      <c r="E31" s="32"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="3">
         <v>7.3</v>
       </c>
@@ -2067,10 +2203,10 @@
       <c r="D32" s="3">
         <v>3</v>
       </c>
-      <c r="E32" s="33"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="35" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="3">
@@ -2079,70 +2215,70 @@
       <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="35">
         <v>6</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="3">
         <v>8.1999999999999993</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="A35" s="33"/>
       <c r="B35" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="A36" s="33"/>
       <c r="B36" s="3">
         <v>8.4</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+      <c r="A37" s="33"/>
       <c r="B37" s="3">
         <v>8.5</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="3">
         <v>8.6</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="32"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="33"/>
     </row>
     <row r="39" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="35" t="s">
         <v>53</v>
       </c>
       <c r="B39" s="3">
@@ -2151,68 +2287,68 @@
       <c r="C39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="31">
+      <c r="D39" s="35">
         <v>6</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="3">
         <v>9.1999999999999993</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
     </row>
     <row r="41" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="3">
         <v>9.3000000000000007</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
     </row>
     <row r="42" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="A42" s="33"/>
       <c r="B42" s="3">
         <v>9.4</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="3">
         <v>9.5</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="3">
         <v>9.6</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="33"/>
-      <c r="E44" s="32"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B45" s="3">
@@ -2221,68 +2357,68 @@
       <c r="C45" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="31">
+      <c r="D45" s="35">
         <v>6</v>
       </c>
-      <c r="E45" s="32"/>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="3">
         <v>10.199999999999999</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="3">
         <v>10.3</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="3">
         <v>10.4</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="3">
         <v>10.5</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
     </row>
     <row r="50" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="3">
         <v>10.6</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="33"/>
-      <c r="E50" s="32"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="33"/>
     </row>
     <row r="51" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B51" s="3">
@@ -2291,35 +2427,35 @@
       <c r="C51" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="31">
+      <c r="D51" s="35">
         <v>6</v>
       </c>
-      <c r="E51" s="32"/>
+      <c r="E51" s="33"/>
     </row>
     <row r="52" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="A52" s="33"/>
       <c r="B52" s="3">
         <v>11.2</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
     </row>
     <row r="53" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
+      <c r="A53" s="34"/>
       <c r="B53" s="3">
         <v>11.3</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="35" t="s">
         <v>71</v>
       </c>
       <c r="B54" s="3">
@@ -2328,81 +2464,81 @@
       <c r="C54" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="31">
+      <c r="D54" s="35">
         <v>6</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E54" s="35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="32"/>
+      <c r="A55" s="33"/>
       <c r="B55" s="3">
         <v>12.2</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+      <c r="A56" s="33"/>
       <c r="B56" s="3">
         <v>12.3</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
+      <c r="A57" s="33"/>
       <c r="B57" s="3">
         <v>12.4</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
+      <c r="A58" s="33"/>
       <c r="B58" s="3">
         <v>12.5</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
     </row>
     <row r="59" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
+      <c r="A59" s="33"/>
       <c r="B59" s="3">
         <v>12.6</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
     </row>
     <row r="60" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="34"/>
       <c r="B60" s="3">
         <v>12.7</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B61" s="3">
@@ -2411,92 +2547,92 @@
       <c r="C61" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="31">
+      <c r="D61" s="35">
         <v>6</v>
       </c>
-      <c r="E61" s="31" t="s">
+      <c r="E61" s="35" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
+      <c r="A62" s="33"/>
       <c r="B62" s="3">
         <v>13.2</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
+      <c r="A63" s="33"/>
       <c r="B63" s="3">
         <v>13.3</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
     </row>
     <row r="64" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
+      <c r="A64" s="33"/>
       <c r="B64" s="3">
         <v>13.4</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
     </row>
     <row r="65" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
+      <c r="A65" s="33"/>
       <c r="B65" s="3">
         <v>13.5</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
     </row>
     <row r="66" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+      <c r="A66" s="33"/>
       <c r="B66" s="3">
         <v>13.6</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
     </row>
     <row r="67" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="32"/>
+      <c r="A67" s="33"/>
       <c r="B67" s="3">
         <v>13.7</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
+      <c r="A68" s="34"/>
       <c r="B68" s="3">
         <v>13.8</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D68" s="33"/>
-      <c r="E68" s="33"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B69" s="3">
@@ -2508,12 +2644,12 @@
       <c r="D69" s="3">
         <v>3</v>
       </c>
-      <c r="E69" s="34" t="s">
+      <c r="E69" s="32" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
+      <c r="A70" s="33"/>
       <c r="B70" s="3">
         <v>14.2</v>
       </c>
@@ -2523,10 +2659,10 @@
       <c r="D70" s="3">
         <v>3</v>
       </c>
-      <c r="E70" s="32"/>
+      <c r="E70" s="33"/>
     </row>
     <row r="71" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
+      <c r="A71" s="33"/>
       <c r="B71" s="3">
         <v>14.3</v>
       </c>
@@ -2536,10 +2672,10 @@
       <c r="D71" s="3">
         <v>2</v>
       </c>
-      <c r="E71" s="32"/>
+      <c r="E71" s="33"/>
     </row>
     <row r="72" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="32"/>
+      <c r="A72" s="33"/>
       <c r="B72" s="3">
         <v>14.4</v>
       </c>
@@ -2549,10 +2685,10 @@
       <c r="D72" s="3">
         <v>2</v>
       </c>
-      <c r="E72" s="32"/>
+      <c r="E72" s="33"/>
     </row>
     <row r="73" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="32"/>
+      <c r="A73" s="33"/>
       <c r="B73" s="3">
         <v>14.5</v>
       </c>
@@ -2562,10 +2698,10 @@
       <c r="D73" s="3">
         <v>2</v>
       </c>
-      <c r="E73" s="32"/>
+      <c r="E73" s="33"/>
     </row>
     <row r="74" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
+      <c r="A74" s="34"/>
       <c r="B74" s="3">
         <v>14.6</v>
       </c>
@@ -2575,7 +2711,7 @@
       <c r="D74" s="3">
         <v>3</v>
       </c>
-      <c r="E74" s="32"/>
+      <c r="E74" s="33"/>
     </row>
     <row r="75" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -2590,10 +2726,10 @@
       <c r="D75" s="3">
         <v>4</v>
       </c>
-      <c r="E75" s="32"/>
+      <c r="E75" s="33"/>
     </row>
     <row r="76" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="35" t="s">
         <v>100</v>
       </c>
       <c r="B76" s="3">
@@ -2605,10 +2741,10 @@
       <c r="D76" s="3">
         <v>3</v>
       </c>
-      <c r="E76" s="32"/>
+      <c r="E76" s="33"/>
     </row>
     <row r="77" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="3">
         <v>15.2</v>
       </c>
@@ -2618,10 +2754,10 @@
       <c r="D77" s="3">
         <v>3</v>
       </c>
-      <c r="E77" s="32"/>
+      <c r="E77" s="33"/>
     </row>
     <row r="78" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="32"/>
+      <c r="A78" s="33"/>
       <c r="B78" s="3">
         <v>15.3</v>
       </c>
@@ -2631,10 +2767,10 @@
       <c r="D78" s="3">
         <v>3</v>
       </c>
-      <c r="E78" s="32"/>
+      <c r="E78" s="33"/>
     </row>
     <row r="79" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="32"/>
+      <c r="A79" s="33"/>
       <c r="B79" s="3">
         <v>15.4</v>
       </c>
@@ -2644,10 +2780,10 @@
       <c r="D79" s="3">
         <v>3</v>
       </c>
-      <c r="E79" s="32"/>
+      <c r="E79" s="33"/>
     </row>
     <row r="80" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+      <c r="A80" s="33"/>
       <c r="B80" s="3">
         <v>15.5</v>
       </c>
@@ -2657,10 +2793,10 @@
       <c r="D80" s="3">
         <v>3</v>
       </c>
-      <c r="E80" s="32"/>
+      <c r="E80" s="33"/>
     </row>
     <row r="81" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
+      <c r="A81" s="34"/>
       <c r="B81" s="3">
         <v>15.6</v>
       </c>
@@ -2670,7 +2806,7 @@
       <c r="D81" s="3">
         <v>3</v>
       </c>
-      <c r="E81" s="32"/>
+      <c r="E81" s="33"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
@@ -2685,10 +2821,10 @@
       <c r="D82" s="3">
         <v>4</v>
       </c>
-      <c r="E82" s="33"/>
+      <c r="E82" s="34"/>
     </row>
     <row r="83" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A83" s="31" t="s">
+      <c r="A83" s="35" t="s">
         <v>108</v>
       </c>
       <c r="B83" s="3">
@@ -2697,48 +2833,48 @@
       <c r="C83" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="31">
+      <c r="D83" s="35">
         <v>6</v>
       </c>
-      <c r="E83" s="34" t="s">
+      <c r="E83" s="32" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="32"/>
+      <c r="A84" s="33"/>
       <c r="B84" s="3">
         <v>16.2</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="32"/>
+      <c r="A85" s="33"/>
       <c r="B85" s="3">
         <v>16.3</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="33"/>
+      <c r="A86" s="34"/>
       <c r="B86" s="3">
         <v>16.399999999999999</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D86" s="33"/>
-      <c r="E86" s="32"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="33"/>
     </row>
     <row r="87" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A87" s="31" t="s">
+      <c r="A87" s="35" t="s">
         <v>114</v>
       </c>
       <c r="B87" s="3">
@@ -2750,10 +2886,10 @@
       <c r="D87" s="3">
         <v>3</v>
       </c>
-      <c r="E87" s="32"/>
+      <c r="E87" s="33"/>
     </row>
     <row r="88" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="32"/>
+      <c r="A88" s="33"/>
       <c r="B88" s="3">
         <v>17.2</v>
       </c>
@@ -2763,10 +2899,10 @@
       <c r="D88" s="3">
         <v>3</v>
       </c>
-      <c r="E88" s="32"/>
+      <c r="E88" s="33"/>
     </row>
     <row r="89" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="33"/>
+      <c r="A89" s="34"/>
       <c r="B89" s="3">
         <v>17.3</v>
       </c>
@@ -2776,7 +2912,7 @@
       <c r="D89" s="3">
         <v>3</v>
       </c>
-      <c r="E89" s="32"/>
+      <c r="E89" s="33"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
@@ -2791,10 +2927,10 @@
       <c r="D90" s="3">
         <v>4</v>
       </c>
-      <c r="E90" s="33"/>
+      <c r="E90" s="34"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="31" t="s">
+      <c r="A91" s="35" t="s">
         <v>119</v>
       </c>
       <c r="B91" s="3">
@@ -2803,81 +2939,81 @@
       <c r="C91" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D91" s="31">
+      <c r="D91" s="35">
         <v>6</v>
       </c>
-      <c r="E91" s="34" t="s">
+      <c r="E91" s="32" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="32"/>
+      <c r="A92" s="33"/>
       <c r="B92" s="3">
         <v>18.2</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
+      <c r="D92" s="33"/>
+      <c r="E92" s="33"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
+      <c r="A93" s="33"/>
       <c r="B93" s="3">
         <v>18.3</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="33"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="32"/>
+      <c r="A94" s="33"/>
       <c r="B94" s="3">
         <v>18.399999999999999</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
     </row>
     <row r="95" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
+      <c r="A95" s="33"/>
       <c r="B95" s="3">
         <v>18.5</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D95" s="32"/>
-      <c r="E95" s="32"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="33"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="32"/>
+      <c r="A96" s="33"/>
       <c r="B96" s="3">
         <v>18.600000000000001</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
     </row>
     <row r="97" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
+      <c r="A97" s="34"/>
       <c r="B97" s="3">
         <v>18.7</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D97" s="33"/>
-      <c r="E97" s="32"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="33"/>
     </row>
     <row r="98" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="31" t="s">
+      <c r="A98" s="35" t="s">
         <v>128</v>
       </c>
       <c r="B98" s="3">
@@ -2886,35 +3022,35 @@
       <c r="C98" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D98" s="31">
-        <v>3</v>
-      </c>
-      <c r="E98" s="32"/>
+      <c r="D98" s="35">
+        <v>3</v>
+      </c>
+      <c r="E98" s="33"/>
     </row>
     <row r="99" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
+      <c r="A99" s="33"/>
       <c r="B99" s="3">
         <v>19.2</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D99" s="32"/>
-      <c r="E99" s="32"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="33"/>
     </row>
     <row r="100" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="33"/>
+      <c r="A100" s="34"/>
       <c r="B100" s="3">
         <v>19.3</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D100" s="33"/>
-      <c r="E100" s="33"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="34"/>
     </row>
     <row r="101" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="31" t="s">
+      <c r="A101" s="35" t="s">
         <v>132</v>
       </c>
       <c r="B101" s="3">
@@ -2923,37 +3059,37 @@
       <c r="C101" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D101" s="31">
-        <v>3</v>
-      </c>
-      <c r="E101" s="34" t="s">
+      <c r="D101" s="35">
+        <v>3</v>
+      </c>
+      <c r="E101" s="32" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="32"/>
+      <c r="A102" s="33"/>
       <c r="B102" s="3">
         <v>20.2</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D102" s="32"/>
-      <c r="E102" s="32"/>
+      <c r="D102" s="33"/>
+      <c r="E102" s="33"/>
     </row>
     <row r="103" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="33"/>
+      <c r="A103" s="34"/>
       <c r="B103" s="3">
         <v>20.3</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D103" s="33"/>
-      <c r="E103" s="32"/>
+      <c r="D103" s="34"/>
+      <c r="E103" s="33"/>
     </row>
     <row r="104" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="31" t="s">
+      <c r="A104" s="35" t="s">
         <v>137</v>
       </c>
       <c r="B104" s="3">
@@ -2962,57 +3098,57 @@
       <c r="C104" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D104" s="31">
+      <c r="D104" s="35">
         <v>6</v>
       </c>
-      <c r="E104" s="32"/>
+      <c r="E104" s="33"/>
     </row>
     <row r="105" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="32"/>
+      <c r="A105" s="33"/>
       <c r="B105" s="3">
         <v>21.2</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D105" s="32"/>
-      <c r="E105" s="32"/>
+      <c r="D105" s="33"/>
+      <c r="E105" s="33"/>
     </row>
     <row r="106" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="32"/>
+      <c r="A106" s="33"/>
       <c r="B106" s="3">
         <v>21.3</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D106" s="32"/>
-      <c r="E106" s="32"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="33"/>
     </row>
     <row r="107" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="32"/>
+      <c r="A107" s="33"/>
       <c r="B107" s="3">
         <v>21.4</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
+      <c r="D107" s="33"/>
+      <c r="E107" s="33"/>
     </row>
     <row r="108" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="33"/>
+      <c r="A108" s="34"/>
       <c r="B108" s="3">
         <v>21.5</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D108" s="33"/>
-      <c r="E108" s="33"/>
+      <c r="D108" s="34"/>
+      <c r="E108" s="34"/>
     </row>
     <row r="109" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="31" t="s">
+      <c r="A109" s="35" t="s">
         <v>143</v>
       </c>
       <c r="B109" s="3">
@@ -3021,59 +3157,59 @@
       <c r="C109" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D109" s="31">
+      <c r="D109" s="35">
         <v>6</v>
       </c>
-      <c r="E109" s="34" t="s">
+      <c r="E109" s="32" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="32"/>
+      <c r="A110" s="33"/>
       <c r="B110" s="3">
         <v>22.2</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D110" s="32"/>
-      <c r="E110" s="32"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="33"/>
     </row>
     <row r="111" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="32"/>
+      <c r="A111" s="33"/>
       <c r="B111" s="3">
         <v>22.3</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D111" s="32"/>
-      <c r="E111" s="32"/>
+      <c r="D111" s="33"/>
+      <c r="E111" s="33"/>
     </row>
     <row r="112" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="32"/>
+      <c r="A112" s="33"/>
       <c r="B112" s="3">
         <v>22.4</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D112" s="32"/>
-      <c r="E112" s="32"/>
+      <c r="D112" s="33"/>
+      <c r="E112" s="33"/>
     </row>
     <row r="113" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="33"/>
+      <c r="A113" s="34"/>
       <c r="B113" s="3">
         <v>22.5</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D113" s="33"/>
-      <c r="E113" s="32"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="33"/>
     </row>
     <row r="114" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="31" t="s">
+      <c r="A114" s="35" t="s">
         <v>150</v>
       </c>
       <c r="B114" s="3">
@@ -3082,43 +3218,43 @@
       <c r="C114" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D114" s="31">
+      <c r="D114" s="35">
         <v>6</v>
       </c>
-      <c r="E114" s="32"/>
+      <c r="E114" s="33"/>
     </row>
     <row r="115" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="32"/>
+      <c r="A115" s="33"/>
       <c r="B115" s="3">
         <v>23.2</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D115" s="32"/>
-      <c r="E115" s="32"/>
+      <c r="D115" s="33"/>
+      <c r="E115" s="33"/>
     </row>
     <row r="116" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="32"/>
+      <c r="A116" s="33"/>
       <c r="B116" s="3">
         <v>23.3</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D116" s="32"/>
-      <c r="E116" s="32"/>
+      <c r="D116" s="33"/>
+      <c r="E116" s="33"/>
     </row>
     <row r="117" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="33"/>
+      <c r="A117" s="34"/>
       <c r="B117" s="3">
         <v>23.4</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D117" s="33"/>
-      <c r="E117" s="32"/>
+      <c r="D117" s="34"/>
+      <c r="E117" s="33"/>
     </row>
     <row r="118" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
@@ -3133,10 +3269,10 @@
       <c r="D118" s="3">
         <v>3</v>
       </c>
-      <c r="E118" s="33"/>
+      <c r="E118" s="34"/>
     </row>
     <row r="119" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="31" t="s">
+      <c r="A119" s="35" t="s">
         <v>156</v>
       </c>
       <c r="B119" s="3">
@@ -3145,70 +3281,70 @@
       <c r="C119" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D119" s="31">
+      <c r="D119" s="35">
         <v>6</v>
       </c>
-      <c r="E119" s="34" t="s">
+      <c r="E119" s="32" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+      <c r="A120" s="33"/>
       <c r="B120" s="3">
         <v>24.2</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D120" s="32"/>
-      <c r="E120" s="32"/>
+      <c r="D120" s="33"/>
+      <c r="E120" s="33"/>
     </row>
     <row r="121" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="32"/>
+      <c r="A121" s="33"/>
       <c r="B121" s="3">
         <v>24.3</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
+      <c r="D121" s="33"/>
+      <c r="E121" s="33"/>
     </row>
     <row r="122" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="32"/>
+      <c r="A122" s="33"/>
       <c r="B122" s="3">
         <v>24.4</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
+      <c r="D122" s="33"/>
+      <c r="E122" s="33"/>
     </row>
     <row r="123" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="32"/>
+      <c r="A123" s="33"/>
       <c r="B123" s="3">
         <v>24.5</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D123" s="32"/>
-      <c r="E123" s="32"/>
+      <c r="D123" s="33"/>
+      <c r="E123" s="33"/>
     </row>
     <row r="124" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A124" s="33"/>
+      <c r="A124" s="34"/>
       <c r="B124" s="3">
         <v>24.6</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D124" s="33"/>
-      <c r="E124" s="32"/>
+      <c r="D124" s="34"/>
+      <c r="E124" s="33"/>
     </row>
     <row r="125" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="31" t="s">
+      <c r="A125" s="35" t="s">
         <v>164</v>
       </c>
       <c r="B125" s="3">
@@ -3217,35 +3353,35 @@
       <c r="C125" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D125" s="31">
+      <c r="D125" s="35">
         <v>6</v>
       </c>
-      <c r="E125" s="32"/>
+      <c r="E125" s="33"/>
     </row>
     <row r="126" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A126" s="32"/>
+      <c r="A126" s="33"/>
       <c r="B126" s="3">
         <v>25.2</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D126" s="32"/>
-      <c r="E126" s="32"/>
+      <c r="D126" s="33"/>
+      <c r="E126" s="33"/>
     </row>
     <row r="127" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="32"/>
+      <c r="A127" s="33"/>
       <c r="B127" s="3">
         <v>25.3</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D127" s="33"/>
-      <c r="E127" s="32"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="33"/>
     </row>
     <row r="128" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="33"/>
+      <c r="A128" s="34"/>
       <c r="B128" s="3">
         <v>25.4</v>
       </c>
@@ -3255,10 +3391,10 @@
       <c r="D128" s="3">
         <v>3</v>
       </c>
-      <c r="E128" s="33"/>
+      <c r="E128" s="34"/>
     </row>
     <row r="129" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="31" t="s">
+      <c r="A129" s="35" t="s">
         <v>169</v>
       </c>
       <c r="B129" s="3">
@@ -3267,37 +3403,37 @@
       <c r="C129" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D129" s="31">
+      <c r="D129" s="35">
         <v>6</v>
       </c>
-      <c r="E129" s="31" t="s">
+      <c r="E129" s="35" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+      <c r="A130" s="33"/>
       <c r="B130" s="3">
         <v>26.2</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D130" s="32"/>
-      <c r="E130" s="32"/>
+      <c r="D130" s="33"/>
+      <c r="E130" s="33"/>
     </row>
     <row r="131" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="33"/>
+      <c r="A131" s="34"/>
       <c r="B131" s="3">
         <v>26.3</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D131" s="33"/>
-      <c r="E131" s="33"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="34"/>
     </row>
     <row r="132" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="31" t="s">
+      <c r="A132" s="35" t="s">
         <v>174</v>
       </c>
       <c r="B132" s="3">
@@ -3309,12 +3445,12 @@
       <c r="D132" s="3">
         <v>5</v>
       </c>
-      <c r="E132" s="34" t="s">
+      <c r="E132" s="32" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A133" s="33"/>
+      <c r="A133" s="34"/>
       <c r="B133" s="3">
         <v>27.2</v>
       </c>
@@ -3324,10 +3460,58 @@
       <c r="D133" s="3">
         <v>10</v>
       </c>
-      <c r="E133" s="33"/>
+      <c r="E133" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E33:E53"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E20"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D119:D124"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E119:E128"/>
+    <mergeCell ref="A125:A128"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="E129:E131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A119:A124"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="D91:D97"/>
+    <mergeCell ref="E91:E100"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="E101:E108"/>
+    <mergeCell ref="D109:D113"/>
+    <mergeCell ref="E109:E118"/>
+    <mergeCell ref="D114:D117"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="A61:A68"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A91:A97"/>
+    <mergeCell ref="A76:A81"/>
     <mergeCell ref="E83:E90"/>
     <mergeCell ref="A87:A89"/>
     <mergeCell ref="D83:D86"/>
@@ -3344,54 +3528,6 @@
     <mergeCell ref="E61:E68"/>
     <mergeCell ref="E69:E82"/>
     <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A68"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A91:A97"/>
-    <mergeCell ref="A76:A81"/>
-    <mergeCell ref="A114:A117"/>
-    <mergeCell ref="E101:E108"/>
-    <mergeCell ref="D109:D113"/>
-    <mergeCell ref="E109:E118"/>
-    <mergeCell ref="D114:D117"/>
-    <mergeCell ref="D101:D103"/>
-    <mergeCell ref="D104:D108"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="D91:D97"/>
-    <mergeCell ref="E91:E100"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="D98:D100"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="D119:D124"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E119:E128"/>
-    <mergeCell ref="A125:A128"/>
-    <mergeCell ref="D125:D127"/>
-    <mergeCell ref="D129:D131"/>
-    <mergeCell ref="E129:E131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A119:A124"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E20"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E33:E53"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="D51:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3401,8 +3537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE790FB6-A56C-104E-ADFC-0FABBBB49FA5}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="G21" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.25"/>
@@ -3415,8 +3551,8 @@
     <col min="7" max="7" width="37.90625" style="5" customWidth="1"/>
     <col min="8" max="8" width="69.36328125" style="5" customWidth="1"/>
     <col min="9" max="9" width="17.36328125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="5"/>
-    <col min="11" max="11" width="13.90625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="16" style="5" customWidth="1"/>
     <col min="12" max="12" width="10.81640625" style="5"/>
     <col min="13" max="13" width="12.54296875" style="5" customWidth="1"/>
     <col min="14" max="16384" width="10.81640625" style="5"/>
@@ -3467,7 +3603,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
+      <c r="A2" s="56">
         <v>1</v>
       </c>
       <c r="B2" s="10">
@@ -3485,16 +3621,16 @@
       <c r="F2" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="36" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="40"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="8">
         <v>44765</v>
       </c>
@@ -3510,14 +3646,14 @@
       <c r="F3" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="44"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="I3" s="40"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:14" ht="23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="8">
         <v>44766</v>
       </c>
@@ -3533,14 +3669,14 @@
       <c r="F4" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="44"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="I4" s="40"/>
+      <c r="I4" s="55"/>
     </row>
     <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
+      <c r="A5" s="57">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3558,7 +3694,7 @@
       <c r="F5" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="38" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="21" t="s">
@@ -3566,7 +3702,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="6" t="s">
         <v>186</v>
       </c>
@@ -3582,13 +3718,13 @@
       <c r="F6" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="21" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="6" t="s">
         <v>187</v>
       </c>
@@ -3604,7 +3740,7 @@
       <c r="F7" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="21" t="s">
@@ -3612,7 +3748,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
+      <c r="A8" s="57">
         <v>3</v>
       </c>
       <c r="B8" s="9">
@@ -3630,13 +3766,13 @@
       <c r="F8" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="21" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="9">
         <v>44720</v>
       </c>
@@ -3652,7 +3788,7 @@
       <c r="F9" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G9" s="42"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="22" t="s">
         <v>240</v>
       </c>
@@ -3677,7 +3813,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="9">
         <v>44750</v>
       </c>
@@ -3693,7 +3829,7 @@
       <c r="F10" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="39" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="22" t="s">
@@ -3720,7 +3856,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+      <c r="A11" s="57">
         <v>4</v>
       </c>
       <c r="B11" s="9">
@@ -3738,7 +3874,7 @@
       <c r="F11" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="42"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="22" t="s">
         <v>243</v>
       </c>
@@ -3763,7 +3899,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="6" t="s">
         <v>188</v>
       </c>
@@ -3779,7 +3915,7 @@
       <c r="F12" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="39" t="s">
         <v>247</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -3798,7 +3934,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="6" t="s">
         <v>189</v>
       </c>
@@ -3814,7 +3950,7 @@
       <c r="F13" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="15" t="s">
         <v>248</v>
       </c>
@@ -3831,7 +3967,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
+      <c r="A14" s="57">
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3849,7 +3985,7 @@
       <c r="F14" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="40" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="15" t="s">
@@ -3868,7 +4004,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="6" t="s">
         <v>191</v>
       </c>
@@ -3884,7 +4020,7 @@
       <c r="F15" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G15" s="48"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="15" t="s">
         <v>40</v>
       </c>
@@ -3901,7 +4037,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="6" t="s">
         <v>192</v>
       </c>
@@ -3917,7 +4053,7 @@
       <c r="F16" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="39" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="23" t="s">
@@ -3936,7 +4072,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
+      <c r="A17" s="57">
         <v>6</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -3954,7 +4090,7 @@
       <c r="F17" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G17" s="42"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="23" t="s">
         <v>43</v>
       </c>
@@ -3971,7 +4107,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="6" t="s">
         <v>194</v>
       </c>
@@ -3987,8 +4123,8 @@
       <c r="F18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="49" t="s">
+      <c r="G18" s="39"/>
+      <c r="H18" s="41" t="s">
         <v>251</v>
       </c>
       <c r="I18" s="27"/>
@@ -4004,7 +4140,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="6" t="s">
         <v>195</v>
       </c>
@@ -4020,8 +4156,8 @@
       <c r="F19" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="50"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="42"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27" t="s">
         <v>178</v>
@@ -4035,7 +4171,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
+      <c r="A20" s="57">
         <v>7</v>
       </c>
       <c r="B20" s="9">
@@ -4053,7 +4189,7 @@
       <c r="F20" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H20" s="24" t="s">
@@ -4080,7 +4216,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="9">
         <v>44629</v>
       </c>
@@ -4096,7 +4232,7 @@
       <c r="F21" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G21" s="42"/>
+      <c r="G21" s="39"/>
       <c r="H21" s="24" t="s">
         <v>253</v>
       </c>
@@ -4121,7 +4257,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="9">
         <v>44660</v>
       </c>
@@ -4137,7 +4273,7 @@
       <c r="F22" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="G22" s="39" t="s">
         <v>60</v>
       </c>
       <c r="H22" s="24" t="s">
@@ -4170,8 +4306,8 @@
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="51" t="s">
+      <c r="G23" s="39"/>
+      <c r="H23" s="43" t="s">
         <v>255</v>
       </c>
       <c r="I23" s="26">
@@ -4195,7 +4331,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="35">
+      <c r="A24" s="57">
         <v>8</v>
       </c>
       <c r="B24" s="9">
@@ -4213,8 +4349,8 @@
       <c r="F24" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="52"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="44"/>
       <c r="I24" s="26">
         <v>44791</v>
       </c>
@@ -4236,7 +4372,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="9">
         <v>44843</v>
       </c>
@@ -4252,7 +4388,7 @@
       <c r="F25" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G25" s="55" t="s">
+      <c r="G25" s="48" t="s">
         <v>71</v>
       </c>
       <c r="H25" s="24" t="s">
@@ -4279,14 +4415,14 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="9"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="51" t="s">
+      <c r="G26" s="49"/>
+      <c r="H26" s="43" t="s">
         <v>259</v>
       </c>
       <c r="I26" s="26">
@@ -4305,19 +4441,19 @@
         <v>0</v>
       </c>
       <c r="N26" s="27">
-        <f t="shared" ref="N26:N31" si="1">L26+M26</f>
+        <f t="shared" ref="N26:N32" si="1">L26+M26</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="9"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="57"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="50"/>
       <c r="I27" s="26">
         <v>44797</v>
       </c>
@@ -4339,7 +4475,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="9">
         <v>44874</v>
       </c>
@@ -4355,9 +4491,9 @@
       <c r="F28" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G28" s="53"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="58">
+      <c r="G28" s="36"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="31">
         <v>44798</v>
       </c>
       <c r="J28" s="27" t="s">
@@ -4378,7 +4514,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A29" s="35">
+      <c r="A29" s="57">
         <v>9</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -4396,7 +4532,7 @@
       <c r="F29" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G29" s="42" t="s">
+      <c r="G29" s="39" t="s">
         <v>80</v>
       </c>
       <c r="H29" s="24" t="s">
@@ -4423,7 +4559,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="6" t="s">
         <v>197</v>
       </c>
@@ -4439,13 +4575,19 @@
       <c r="F30" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G30" s="42"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
+      <c r="I30" s="26">
+        <v>44803</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="K30" s="27" t="s">
+        <v>306</v>
+      </c>
       <c r="L30" s="27">
         <v>2.5</v>
       </c>
@@ -4458,7 +4600,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="57"/>
       <c r="B31" s="6" t="s">
         <v>198</v>
       </c>
@@ -4474,15 +4616,21 @@
       <c r="F31" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G31" s="42" t="s">
+      <c r="G31" s="39" t="s">
         <v>90</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
+      <c r="I31" s="26">
+        <v>44805</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="K31" s="27" t="s">
+        <v>306</v>
+      </c>
       <c r="L31" s="27">
         <v>2.5</v>
       </c>
@@ -4495,7 +4643,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="35">
+      <c r="A32" s="57">
         <v>10</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -4513,19 +4661,31 @@
       <c r="F32" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G32" s="44"/>
+      <c r="G32" s="37"/>
       <c r="H32" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
+      <c r="I32" s="26">
+        <v>44809</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="L32" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="M32" s="27">
+        <v>0</v>
+      </c>
+      <c r="N32" s="27">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="57"/>
       <c r="B33" s="6" t="s">
         <v>200</v>
       </c>
@@ -4541,7 +4701,7 @@
       <c r="F33" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G33" s="44"/>
+      <c r="G33" s="37"/>
       <c r="H33" s="24" t="s">
         <v>94</v>
       </c>
@@ -4553,7 +4713,7 @@
       <c r="N33" s="27"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="57"/>
       <c r="B34" s="6" t="s">
         <v>201</v>
       </c>
@@ -4569,7 +4729,7 @@
       <c r="F34" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G34" s="44"/>
+      <c r="G34" s="37"/>
       <c r="H34" s="24" t="s">
         <v>95</v>
       </c>
@@ -4581,7 +4741,7 @@
       <c r="N34" s="27"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="35">
+      <c r="A35" s="57">
         <v>11</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -4599,7 +4759,7 @@
       <c r="F35" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G35" s="44"/>
+      <c r="G35" s="37"/>
       <c r="H35" s="24" t="s">
         <v>96</v>
       </c>
@@ -4611,7 +4771,7 @@
       <c r="N35" s="27"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="57"/>
       <c r="B36" s="9">
         <v>44571</v>
       </c>
@@ -4627,7 +4787,7 @@
       <c r="F36" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G36" s="44"/>
+      <c r="G36" s="37"/>
       <c r="H36" s="24" t="s">
         <v>97</v>
       </c>
@@ -4639,7 +4799,7 @@
       <c r="N36" s="27"/>
     </row>
     <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="57"/>
       <c r="B37" s="9">
         <v>44602</v>
       </c>
@@ -4669,7 +4829,7 @@
       <c r="N37" s="27"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="35">
+      <c r="A38" s="57">
         <v>12</v>
       </c>
       <c r="B38" s="9">
@@ -4687,7 +4847,7 @@
       <c r="F38" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G38" s="42" t="s">
+      <c r="G38" s="39" t="s">
         <v>100</v>
       </c>
       <c r="H38" s="24" t="s">
@@ -4701,7 +4861,7 @@
       <c r="N38" s="27"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="9">
         <v>44783</v>
       </c>
@@ -4717,7 +4877,7 @@
       <c r="F39" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G39" s="42"/>
+      <c r="G39" s="39"/>
       <c r="H39" s="24" t="s">
         <v>273</v>
       </c>
@@ -4729,7 +4889,7 @@
       <c r="N39" s="27"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="9">
         <v>44814</v>
       </c>
@@ -4745,7 +4905,7 @@
       <c r="F40" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G40" s="42"/>
+      <c r="G40" s="39"/>
       <c r="H40" s="24" t="s">
         <v>104</v>
       </c>
@@ -4757,7 +4917,7 @@
       <c r="N40" s="27"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="35">
+      <c r="A41" s="57">
         <v>13</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -4775,7 +4935,7 @@
       <c r="F41" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G41" s="42"/>
+      <c r="G41" s="39"/>
       <c r="H41" s="24" t="s">
         <v>105</v>
       </c>
@@ -4787,7 +4947,7 @@
       <c r="N41" s="27"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="57"/>
       <c r="B42" s="6" t="s">
         <v>204</v>
       </c>
@@ -4803,7 +4963,7 @@
       <c r="F42" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G42" s="42"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="24" t="s">
         <v>106</v>
       </c>
@@ -4815,7 +4975,7 @@
       <c r="N42" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="6" t="s">
         <v>205</v>
       </c>
@@ -4831,7 +4991,7 @@
       <c r="F43" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G43" s="42"/>
+      <c r="G43" s="39"/>
       <c r="H43" s="24" t="s">
         <v>102</v>
       </c>
@@ -4843,7 +5003,7 @@
       <c r="N43" s="27"/>
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35">
+      <c r="A44" s="57">
         <v>14</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -4875,7 +5035,7 @@
       <c r="N44" s="27"/>
     </row>
     <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="6" t="s">
         <v>207</v>
       </c>
@@ -4901,7 +5061,7 @@
       <c r="N45" s="27"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="6" t="s">
         <v>208</v>
       </c>
@@ -4917,7 +5077,7 @@
       <c r="F46" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G46" s="42" t="s">
+      <c r="G46" s="39" t="s">
         <v>108</v>
       </c>
       <c r="H46" s="24" t="s">
@@ -4931,7 +5091,7 @@
       <c r="N46" s="27"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="35">
+      <c r="A47" s="57">
         <v>15</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -4949,7 +5109,7 @@
       <c r="F47" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G47" s="42"/>
+      <c r="G47" s="39"/>
       <c r="H47" s="24" t="s">
         <v>265</v>
       </c>
@@ -4961,7 +5121,7 @@
       <c r="N47" s="27"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="57"/>
       <c r="B48" s="6" t="s">
         <v>210</v>
       </c>
@@ -4977,7 +5137,7 @@
       <c r="F48" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="39" t="s">
         <v>114</v>
       </c>
       <c r="H48" s="24" t="s">
@@ -4991,7 +5151,7 @@
       <c r="N48" s="27"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="57"/>
       <c r="B49" s="6" t="s">
         <v>211</v>
       </c>
@@ -5007,7 +5167,7 @@
       <c r="F49" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G49" s="42"/>
+      <c r="G49" s="39"/>
       <c r="H49" s="24" t="s">
         <v>117</v>
       </c>
@@ -5019,7 +5179,7 @@
       <c r="N49" s="27"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="35">
+      <c r="A50" s="57">
         <v>16</v>
       </c>
       <c r="B50" s="9">
@@ -5037,7 +5197,7 @@
       <c r="F50" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G50" s="42"/>
+      <c r="G50" s="39"/>
       <c r="H50" s="24" t="s">
         <v>116</v>
       </c>
@@ -5049,7 +5209,7 @@
       <c r="N50" s="27"/>
     </row>
     <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+      <c r="A51" s="57"/>
       <c r="B51" s="9">
         <v>44692</v>
       </c>
@@ -5079,7 +5239,7 @@
       <c r="N51" s="27"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="57"/>
       <c r="B52" s="9">
         <v>44723</v>
       </c>
@@ -5095,7 +5255,7 @@
       <c r="F52" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G52" s="42" t="s">
+      <c r="G52" s="39" t="s">
         <v>268</v>
       </c>
       <c r="H52" s="24" t="s">
@@ -5109,7 +5269,7 @@
       <c r="N52" s="27"/>
     </row>
     <row r="53" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35">
+      <c r="A53" s="57">
         <v>17</v>
       </c>
       <c r="B53" s="9">
@@ -5127,7 +5287,7 @@
       <c r="F53" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G53" s="42"/>
+      <c r="G53" s="39"/>
       <c r="H53" s="24" t="s">
         <v>269</v>
       </c>
@@ -5139,7 +5299,7 @@
       <c r="N53" s="27"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+      <c r="A54" s="57"/>
       <c r="B54" s="9">
         <v>44906</v>
       </c>
@@ -5155,7 +5315,7 @@
       <c r="F54" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G54" s="42"/>
+      <c r="G54" s="39"/>
       <c r="H54" s="24" t="s">
         <v>166</v>
       </c>
@@ -5167,7 +5327,7 @@
       <c r="N54" s="27"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
+      <c r="A55" s="57"/>
       <c r="B55" s="6" t="s">
         <v>212</v>
       </c>
@@ -5183,7 +5343,7 @@
       <c r="F55" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G55" s="42"/>
+      <c r="G55" s="39"/>
       <c r="H55" s="24" t="s">
         <v>167</v>
       </c>
@@ -5195,7 +5355,7 @@
       <c r="N55" s="27"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="35">
+      <c r="A56" s="57">
         <v>18</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -5213,7 +5373,7 @@
       <c r="F56" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G56" s="42" t="s">
+      <c r="G56" s="39" t="s">
         <v>271</v>
       </c>
       <c r="H56" s="24" t="s">
@@ -5227,7 +5387,7 @@
       <c r="N56" s="27"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="A57" s="57"/>
       <c r="B57" s="6" t="s">
         <v>214</v>
       </c>
@@ -5243,7 +5403,7 @@
       <c r="F57" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G57" s="42"/>
+      <c r="G57" s="39"/>
       <c r="H57" s="24" t="s">
         <v>274</v>
       </c>
@@ -5255,7 +5415,7 @@
       <c r="N57" s="27"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="A58" s="57"/>
       <c r="B58" s="6" t="s">
         <v>215</v>
       </c>
@@ -5271,7 +5431,7 @@
       <c r="F58" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G58" s="42"/>
+      <c r="G58" s="39"/>
       <c r="H58" s="24" t="s">
         <v>279</v>
       </c>
@@ -5283,7 +5443,7 @@
       <c r="N58" s="27"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="35">
+      <c r="A59" s="57">
         <v>19</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -5301,7 +5461,7 @@
       <c r="F59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G59" s="42"/>
+      <c r="G59" s="39"/>
       <c r="H59" s="15"/>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
@@ -5311,7 +5471,7 @@
       <c r="N59" s="27"/>
     </row>
     <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="A60" s="57"/>
       <c r="B60" s="6" t="s">
         <v>217</v>
       </c>
@@ -5341,7 +5501,7 @@
       <c r="N60" s="27"/>
     </row>
     <row r="61" spans="1:14" ht="28" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="57"/>
       <c r="B61" s="6" t="s">
         <v>218</v>
       </c>
@@ -5371,7 +5531,7 @@
       <c r="N61" s="27"/>
     </row>
     <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35">
+      <c r="A62" s="57">
         <v>20</v>
       </c>
       <c r="B62" s="9">
@@ -5389,7 +5549,7 @@
       <c r="F62" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G62" s="42" t="s">
+      <c r="G62" s="39" t="s">
         <v>67</v>
       </c>
       <c r="H62" s="15" t="s">
@@ -5403,7 +5563,7 @@
       <c r="N62" s="27"/>
     </row>
     <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
+      <c r="A63" s="57"/>
       <c r="B63" s="9">
         <v>44632</v>
       </c>
@@ -5419,7 +5579,7 @@
       <c r="F63" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G63" s="42"/>
+      <c r="G63" s="39"/>
       <c r="H63" s="15" t="s">
         <v>70</v>
       </c>
@@ -5431,7 +5591,7 @@
       <c r="N63" s="27"/>
     </row>
     <row r="64" spans="1:14" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
+      <c r="A64" s="57"/>
       <c r="B64" s="9">
         <v>44663</v>
       </c>
@@ -5447,7 +5607,7 @@
       <c r="F64" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G64" s="42" t="s">
+      <c r="G64" s="39" t="s">
         <v>119</v>
       </c>
       <c r="H64" s="15" t="s">
@@ -5461,7 +5621,7 @@
       <c r="N64" s="27"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="35">
+      <c r="A65" s="57">
         <v>21</v>
       </c>
       <c r="B65" s="9">
@@ -5479,7 +5639,7 @@
       <c r="F65" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G65" s="42"/>
+      <c r="G65" s="39"/>
       <c r="H65" s="15" t="s">
         <v>278</v>
       </c>
@@ -5491,7 +5651,7 @@
       <c r="N65" s="27"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+      <c r="A66" s="57"/>
       <c r="B66" s="9">
         <v>44846</v>
       </c>
@@ -5521,7 +5681,7 @@
       <c r="N66" s="27"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
+      <c r="A67" s="57"/>
       <c r="B67" s="9">
         <v>44877</v>
       </c>
@@ -5551,7 +5711,7 @@
       <c r="N67" s="27"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="35">
+      <c r="A68" s="57">
         <v>22</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -5569,7 +5729,7 @@
       <c r="F68" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G68" s="42" t="s">
+      <c r="G68" s="39" t="s">
         <v>137</v>
       </c>
       <c r="H68" s="15" t="s">
@@ -5583,7 +5743,7 @@
       <c r="N68" s="27"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
+      <c r="A69" s="57"/>
       <c r="B69" s="6" t="s">
         <v>220</v>
       </c>
@@ -5599,7 +5759,7 @@
       <c r="F69" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G69" s="42"/>
+      <c r="G69" s="39"/>
       <c r="H69" s="15" t="s">
         <v>282</v>
       </c>
@@ -5611,7 +5771,7 @@
       <c r="N69" s="27"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
+      <c r="A70" s="57"/>
       <c r="B70" s="6" t="s">
         <v>221</v>
       </c>
@@ -5627,7 +5787,7 @@
       <c r="F70" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G70" s="42"/>
+      <c r="G70" s="39"/>
       <c r="H70" s="15" t="s">
         <v>283</v>
       </c>
@@ -5639,7 +5799,7 @@
       <c r="N70" s="27"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="35">
+      <c r="A71" s="57">
         <v>23</v>
       </c>
       <c r="B71" s="6" t="s">
@@ -5657,7 +5817,7 @@
       <c r="F71" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G71" s="42" t="s">
+      <c r="G71" s="39" t="s">
         <v>143</v>
       </c>
       <c r="H71" s="15" t="s">
@@ -5671,7 +5831,7 @@
       <c r="N71" s="27"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
+      <c r="A72" s="57"/>
       <c r="B72" s="6" t="s">
         <v>223</v>
       </c>
@@ -5687,7 +5847,7 @@
       <c r="F72" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G72" s="42"/>
+      <c r="G72" s="39"/>
       <c r="H72" s="15" t="s">
         <v>285</v>
       </c>
@@ -5699,7 +5859,7 @@
       <c r="N72" s="27"/>
     </row>
     <row r="73" spans="1:14" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
+      <c r="A73" s="57"/>
       <c r="B73" s="6" t="s">
         <v>224</v>
       </c>
@@ -5715,7 +5875,7 @@
       <c r="F73" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G73" s="42" t="s">
+      <c r="G73" s="39" t="s">
         <v>150</v>
       </c>
       <c r="H73" s="15" t="s">
@@ -5729,7 +5889,7 @@
       <c r="N73" s="27"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="35">
+      <c r="A74" s="57">
         <v>24</v>
       </c>
       <c r="B74" s="6" t="s">
@@ -5747,7 +5907,7 @@
       <c r="F74" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G74" s="42"/>
+      <c r="G74" s="39"/>
       <c r="H74" s="15" t="s">
         <v>287</v>
       </c>
@@ -5759,7 +5919,7 @@
       <c r="N74" s="27"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+      <c r="A75" s="57"/>
       <c r="B75" s="6" t="s">
         <v>226</v>
       </c>
@@ -5789,7 +5949,7 @@
       <c r="N75" s="27"/>
     </row>
     <row r="76" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A76" s="35"/>
+      <c r="A76" s="57"/>
       <c r="B76" s="9">
         <v>44927</v>
       </c>
@@ -5805,7 +5965,7 @@
       <c r="F76" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G76" s="43" t="s">
+      <c r="G76" s="58" t="s">
         <v>156</v>
       </c>
       <c r="H76" s="15" t="s">
@@ -5819,7 +5979,7 @@
       <c r="N76" s="27"/>
     </row>
     <row r="77" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A77" s="35">
+      <c r="A77" s="57">
         <v>25</v>
       </c>
       <c r="B77" s="9">
@@ -5837,7 +5997,7 @@
       <c r="F77" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G77" s="43"/>
+      <c r="G77" s="58"/>
       <c r="H77" s="15" t="s">
         <v>291</v>
       </c>
@@ -5849,7 +6009,7 @@
       <c r="N77" s="27"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" s="35"/>
+      <c r="A78" s="57"/>
       <c r="B78" s="9">
         <v>45108</v>
       </c>
@@ -5865,7 +6025,7 @@
       <c r="F78" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G78" s="42" t="s">
+      <c r="G78" s="39" t="s">
         <v>169</v>
       </c>
       <c r="H78" s="15" t="s">
@@ -5879,7 +6039,7 @@
       <c r="N78" s="27"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" s="35"/>
+      <c r="A79" s="57"/>
       <c r="B79" s="9">
         <v>45139</v>
       </c>
@@ -5895,7 +6055,7 @@
       <c r="F79" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G79" s="44"/>
+      <c r="G79" s="37"/>
       <c r="H79" s="15" t="s">
         <v>172</v>
       </c>
@@ -5907,7 +6067,7 @@
       <c r="N79" s="27"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A80" s="35">
+      <c r="A80" s="57">
         <v>26</v>
       </c>
       <c r="B80" s="6" t="s">
@@ -5925,7 +6085,7 @@
       <c r="F80" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G80" s="44"/>
+      <c r="G80" s="37"/>
       <c r="H80" s="15" t="s">
         <v>173</v>
       </c>
@@ -5937,7 +6097,7 @@
       <c r="N80" s="27"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="35"/>
+      <c r="A81" s="57"/>
       <c r="B81" s="6" t="s">
         <v>228</v>
       </c>
@@ -5953,10 +6113,10 @@
       <c r="F81" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G81" s="39" t="s">
+      <c r="G81" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="H81" s="39" t="s">
+      <c r="H81" s="54" t="s">
         <v>175</v>
       </c>
       <c r="I81" s="27"/>
@@ -5967,7 +6127,7 @@
       <c r="N81" s="27"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="35"/>
+      <c r="A82" s="57"/>
       <c r="B82" s="6" t="s">
         <v>229</v>
       </c>
@@ -5983,8 +6143,8 @@
       <c r="F82" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G82" s="39"/>
-      <c r="H82" s="39"/>
+      <c r="G82" s="54"/>
+      <c r="H82" s="54"/>
       <c r="I82" s="27"/>
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>
@@ -5993,7 +6153,7 @@
       <c r="N82" s="27"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="35">
+      <c r="A83" s="57">
         <v>27</v>
       </c>
       <c r="B83" s="6" t="s">
@@ -6011,8 +6171,8 @@
       <c r="F83" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G83" s="39"/>
-      <c r="H83" s="36" t="s">
+      <c r="G83" s="54"/>
+      <c r="H83" s="51" t="s">
         <v>295</v>
       </c>
       <c r="I83" s="27"/>
@@ -6023,7 +6183,7 @@
       <c r="N83" s="27"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="35"/>
+      <c r="A84" s="57"/>
       <c r="B84" s="6" t="s">
         <v>292</v>
       </c>
@@ -6039,8 +6199,8 @@
       <c r="F84" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G84" s="39"/>
-      <c r="H84" s="37"/>
+      <c r="G84" s="54"/>
+      <c r="H84" s="52"/>
       <c r="I84" s="27"/>
       <c r="J84" s="27"/>
       <c r="K84" s="27"/>
@@ -6049,7 +6209,7 @@
       <c r="N84" s="27"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="35"/>
+      <c r="A85" s="57"/>
       <c r="B85" s="6" t="s">
         <v>293</v>
       </c>
@@ -6065,8 +6225,8 @@
       <c r="F85" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G85" s="39"/>
-      <c r="H85" s="38"/>
+      <c r="G85" s="54"/>
+      <c r="H85" s="53"/>
       <c r="I85" s="27"/>
       <c r="J85" s="27"/>
       <c r="K85" s="27"/>
@@ -6076,30 +6236,26 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="G38:G43"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="G31:G36"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="G56:G59"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G48:G50"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
     <mergeCell ref="H83:H85"/>
     <mergeCell ref="H81:H82"/>
     <mergeCell ref="I2:I4"/>
@@ -6116,26 +6272,30 @@
     <mergeCell ref="G81:G85"/>
     <mergeCell ref="G62:G63"/>
     <mergeCell ref="G64:G65"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="G56:G59"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G48:G50"/>
+    <mergeCell ref="G38:G43"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="G31:G36"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6145,14 +6305,263 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2945019F-8347-42C2-B174-2DCCBC2A5AD3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="62">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="C1" s="62">
+        <v>0.92986111111111114</v>
+      </c>
+      <c r="D1" s="61">
+        <f>C1-B1</f>
+        <v>0.12013888888888891</v>
+      </c>
+      <c r="E1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="61">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="64">
+        <v>0.83263888888888893</v>
+      </c>
+      <c r="C3" s="64">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D3" s="61">
+        <f t="shared" ref="D3:D14" si="0">C3-B3</f>
+        <v>8.4027777777777701E-2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="63" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="64">
+        <v>0.83263888888888893</v>
+      </c>
+      <c r="C4" s="64">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="D4" s="61">
+        <f t="shared" si="0"/>
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="63" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" s="64">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="C5" s="64">
+        <v>0.92083333333333339</v>
+      </c>
+      <c r="D5" s="61">
+        <f t="shared" si="0"/>
+        <v>0.10972222222222239</v>
+      </c>
+      <c r="E5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="63" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="64">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="C6" s="64">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="D6" s="61">
+        <f t="shared" si="0"/>
+        <v>0.10763888888888884</v>
+      </c>
+      <c r="E6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" s="64">
+        <v>0.82361111111111107</v>
+      </c>
+      <c r="C7" s="64">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="D7" s="61">
+        <f t="shared" si="0"/>
+        <v>0.11736111111111114</v>
+      </c>
+      <c r="E7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="63" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="64">
+        <v>0.8222222222222223</v>
+      </c>
+      <c r="C8" s="64">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D8" s="61">
+        <f t="shared" si="0"/>
+        <v>0.10486111111111107</v>
+      </c>
+      <c r="E8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="63" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="65">
+        <v>0.81652777777777785</v>
+      </c>
+      <c r="C9" s="65">
+        <v>0.9331828703703704</v>
+      </c>
+      <c r="D9" s="61">
+        <f t="shared" si="0"/>
+        <v>0.11665509259259255</v>
+      </c>
+      <c r="E9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" s="66">
+        <v>0.82262731481481488</v>
+      </c>
+      <c r="C10" s="65">
+        <v>0.93069444444444438</v>
+      </c>
+      <c r="D10" s="61">
+        <f t="shared" si="0"/>
+        <v>0.1080671296296295</v>
+      </c>
+      <c r="E10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="s">
+        <v>319</v>
+      </c>
+      <c r="B11" s="65">
+        <v>0.82320601851851849</v>
+      </c>
+      <c r="C11" s="65">
+        <v>0.92936342592592591</v>
+      </c>
+      <c r="D11" s="61">
+        <f t="shared" si="0"/>
+        <v>0.10615740740740742</v>
+      </c>
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="63" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" s="66">
+        <v>0.32318287037037036</v>
+      </c>
+      <c r="C12" s="66">
+        <v>0.44081018518518517</v>
+      </c>
+      <c r="D12" s="61">
+        <f t="shared" si="0"/>
+        <v>0.11762731481481481</v>
+      </c>
+      <c r="E12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="63" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="66">
+        <v>0.3127314814814815</v>
+      </c>
+      <c r="C13" s="66">
+        <v>0.43391203703703707</v>
+      </c>
+      <c r="D13" s="61">
+        <f t="shared" si="0"/>
+        <v>0.12118055555555557</v>
+      </c>
+      <c r="E13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="63" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" s="66">
+        <v>0.31361111111111112</v>
+      </c>
+      <c r="C14" s="66">
+        <v>0.4410648148148148</v>
+      </c>
+      <c r="D14" s="61">
+        <f t="shared" si="0"/>
+        <v>0.12745370370370368</v>
+      </c>
+      <c r="E14">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>